<commit_message>
NN Model training update
</commit_message>
<xml_diff>
--- a/ModelingSupportProfiles.xlsx
+++ b/ModelingSupportProfiles.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12030" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="5-13 1130" sheetId="2" r:id="rId1"/>
-    <sheet name="5-15 0830" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="Plot Data" sheetId="5" r:id="rId2"/>
+    <sheet name="5-15 0830" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="46">
   <si>
     <t>Location</t>
   </si>
@@ -141,12 +142,36 @@
   <si>
     <t>Total HRT</t>
   </si>
+  <si>
+    <t>N Dis Outfall Weir Flow (MGD)</t>
+  </si>
+  <si>
+    <t>Double Exponential</t>
+  </si>
+  <si>
+    <t>Single Exponential</t>
+  </si>
+  <si>
+    <t>R sq</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>(integration from 0 to 5 &amp; 5 to 60)</t>
+  </si>
+  <si>
+    <t>Chemscan</t>
+  </si>
+  <si>
+    <t>(integration from 0 to 5 &amp; 5 to 38)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,6 +181,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -371,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -443,18 +476,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -470,6 +491,34 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -504,13 +553,1120 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11316439648979477"/>
+          <c:y val="5.0925925925925923E-2"/>
+          <c:w val="0.85192737312129363"/>
+          <c:h val="0.74350320793234181"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>13-May</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Plot Data'!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8621456672052348</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0134900169257559</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5891621917860164</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.1648343666462768</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.7405065415065373</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.3161787163668</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.46752306608732</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>26.281874757752103</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>38.096226449416889</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Plot Data'!$C$2:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999523162842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-72C4-42D6-A9F0-A4F887D1FA16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>15-May</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Plot Data'!$E$13:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9139740845546025</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.8642753775994958</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10.339426024121941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12.814576670644389</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15.289727317166834</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>17.76487796368928</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22.715179256734174</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.994488967988367</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41.27379867924256</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50.553108390496746</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>59.832418101750925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Plot Data'!$C$13:$C$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999523162842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000009-72C4-42D6-A9F0-A4F887D1FA16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Model 2</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.5904291033388269E-2"/>
+                  <c:y val="-9.3017643627879842E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$E$4:$E$11,'Plot Data'!$E$15:$E$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>5.0134900169257559</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.5891621917860164</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1648343666462768</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7405065415065373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11.3161787163668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.46752306608732</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.281874757752103</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>38.096226449416889</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.8642753775994958</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10.339426024121941</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12.814576670644389</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.289727317166834</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>17.76487796368928</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22.715179256734174</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>31.994488967988367</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>41.27379867924256</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>50.553108390496746</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>59.832418101750925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$C$4:$C$11,'Plot Data'!$C$15:$C$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000B-72C4-42D6-A9F0-A4F887D1FA16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Model 1</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.15026833631484796"/>
+                  <c:y val="-0.14734762321376493"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$E$2:$E$3,'Plot Data'!$E$13,'Plot Data'!$E$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8621456672052348</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9139740845546025</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$C$2,'Plot Data'!$C$3,'Plot Data'!$C$13,'Plot Data'!$C$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.2999999523162842</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2999999523162842</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.82</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000C-72C4-42D6-A9F0-A4F887D1FA16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Model M</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="exp"/>
+            <c:backward val="1.5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.37518703721963198"/>
+                  <c:y val="-0.26878062117235346"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="bg1"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:schemeClr val="accent1"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:sysClr val="windowText" lastClr="000000"/>
+                      </a:solidFill>
+                      <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$E$3:$E$11,'Plot Data'!$E$14:$E$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>1.8621456672052348</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0134900169257559</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5891621917860164</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.1648343666462768</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7405065415065373</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.3161787163668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.46752306608732</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>26.281874757752103</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.096226449416889</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.9139740845546025</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7.8642753775994958</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.339426024121941</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12.814576670644389</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15.289727317166834</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>17.76487796368928</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22.715179256734174</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>31.994488967988367</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>41.27379867924256</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>50.553108390496746</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>59.832418101750925</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$C$3:$C$11,'Plot Data'!$C$14:$C$24)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000000D-72C4-42D6-A9F0-A4F887D1FA16}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>Chemscan</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$E$15,'Plot Data'!$E$4)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>7.8642753775994958</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0134900169257559</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>('Plot Data'!$J$15,'Plot Data'!$J$4)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.48027771711349487</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.54421299695968628</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-86E3-4ED6-B4FA-0D03F72FCAD1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="831056639"/>
+        <c:axId val="831054143"/>
+        <c:extLst/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="831056639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (minutes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.45055446194225723"/>
+              <c:y val="0.90645815106445027"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="in"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="831054143"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:minorUnit val="5"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="831054143"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>PAA Concentration (mg/L)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9444444444444445E-2"/>
+              <c:y val="0.1629666083406241"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="831056639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="2"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72552110771484513"/>
+          <c:y val="4.7452610090405363E-2"/>
+          <c:w val="0.2426597927495199"/>
+          <c:h val="0.36725357247010793"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
         </a:ln>
         <a:effectLst/>
       </c:spPr>
@@ -519,23 +1675,72 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -610,7 +1815,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$6:$F$16</c:f>
+              <c:f>Sheet1!$H$6:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -737,7 +1942,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$6:$G$16</c:f>
+              <c:f>Sheet1!$I$6:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -923,7 +2128,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1030,7 +2234,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1608,6 +3368,41 @@
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>295274</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1666,20 +3461,20 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>89647</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>17929</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>605117</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>186017</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>425823</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>94129</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>336175</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>71717</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1966,8 +3761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C14"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1991,14 +3786,14 @@
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2266,10 +4061,689 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="31" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="41">
+        <v>43598.506944444445</v>
+      </c>
+      <c r="C2" s="45">
+        <f>_xll.PITimeDat("DIS N PAA Target Dose, C",'Plot Data'!$B$2,"\\APPLEPI_AF\MWRD_Production\Hite Treatment Plant\07-Disinfection\Dis_PAA\North_PAA\North_PAA_Dose_Cntrl\CT Dosing Method","interpolated")</f>
+        <v>1.2999999523162842</v>
+      </c>
+      <c r="D2" s="44">
+        <f>AVERAGE(D3:D11)</f>
+        <v>85.970995585123703</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>1.2969*EXP(-0.16*E2)</f>
+        <v>1.2968999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="41">
+        <v>43598.504861111112</v>
+      </c>
+      <c r="C3" s="18">
+        <v>0.95</v>
+      </c>
+      <c r="D3" s="42">
+        <f t="array" ref="D3:D11">_xll.PITimeDat("N CMPLX OUTFALL WEIR (FI-F350)",'Plot Data'!$B$3:$B$11,"\\APPLEPI_AF\MWRD_Production\Hite Treatment Plant\07-Disinfection\Dis_Plant_Flows","interpolated")</f>
+        <v>84.987594604492188</v>
+      </c>
+      <c r="E3" s="44">
+        <v>1.8621456672052348</v>
+      </c>
+      <c r="G3">
+        <f>1.2969*EXP(-0.16*E3)</f>
+        <v>0.96274518712257429</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H11" si="0">0.8711*EXP(-0.029*E3)</f>
+        <v>0.82530627220253328</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="41">
+        <v>43598.502083333333</v>
+      </c>
+      <c r="C4" s="18">
+        <v>0.69</v>
+      </c>
+      <c r="D4" s="42">
+        <v>85.587074279785156</v>
+      </c>
+      <c r="E4">
+        <f>E3+(E6-E3)/2</f>
+        <v>5.0134900169257559</v>
+      </c>
+      <c r="G4">
+        <f>0.8499*EXP(-0.028*E4)</f>
+        <v>0.73858853156040605</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.75322619189400464</v>
+      </c>
+      <c r="J4" s="42">
+        <f t="array" ref="J4">_xll.PITimeDat("AI_K826",'Plot Data'!$B$4,"\\applepi","interpolated")</f>
+        <v>0.54421299695968628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="41">
+        <v>43598.499305555553</v>
+      </c>
+      <c r="C5" s="18">
+        <v>0.69</v>
+      </c>
+      <c r="D5" s="42">
+        <v>85.921409606933594</v>
+      </c>
+      <c r="E5">
+        <f>E4+(E6-E4)/2</f>
+        <v>6.5891621917860164</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ref="G5:G11" si="1">0.8499*EXP(-0.028*E5)</f>
+        <v>0.70671124116897066</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.71958242411897511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="41">
+        <v>43598.496527777781</v>
+      </c>
+      <c r="C6" s="18">
+        <v>0.67</v>
+      </c>
+      <c r="D6" s="42">
+        <v>86.19775390625</v>
+      </c>
+      <c r="E6">
+        <f>E3+(E9-E3)/2</f>
+        <v>8.1648343666462768</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>0.67620976640325725</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.68744139632070334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="41">
+        <v>43598.494444444441</v>
+      </c>
+      <c r="C7" s="18">
+        <v>0.63</v>
+      </c>
+      <c r="D7" s="42">
+        <v>86.383735656738281</v>
+      </c>
+      <c r="E7">
+        <f>E6+(E8-E6)/2</f>
+        <v>9.7405065415065373</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>0.64702472741595973</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.65673598678283318</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="41">
+        <v>43598.493055555555</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.62</v>
+      </c>
+      <c r="D8" s="42">
+        <v>86.397811889648438</v>
+      </c>
+      <c r="E8">
+        <f>E6+(E9-E6)/2</f>
+        <v>11.3161787163668</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>0.61909930717865536</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.62740207186244523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="41">
+        <v>43598.490972222222</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D9" s="42">
+        <v>86.418914794921875</v>
+      </c>
+      <c r="E9" s="44">
+        <v>14.46752306608732</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.56681221004507032</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.57260642417532293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="41">
+        <v>43598.488194444442</v>
+      </c>
+      <c r="C10" s="18">
+        <v>0.47</v>
+      </c>
+      <c r="D10" s="42">
+        <v>86.447059631347656</v>
+      </c>
+      <c r="E10" s="44">
+        <v>26.281874757752103</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.4071681325742878</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.40649938369043931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="41">
+        <v>43598.48333333333</v>
+      </c>
+      <c r="C11" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="D11" s="42">
+        <v>85.397605895996094</v>
+      </c>
+      <c r="E11" s="44">
+        <v>38.096226449416889</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.29248820905049</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.28857823098769952</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="16"/>
+      <c r="D12" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12">
+        <f>4.46353+15.9139</f>
+        <v>20.37743</v>
+      </c>
+      <c r="H12">
+        <v>20.059100000000001</v>
+      </c>
+      <c r="I12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="41">
+        <v>43600.390972222223</v>
+      </c>
+      <c r="C13" s="45">
+        <f t="array" ref="C13">_xll.PITimeDat("DIS N PAA Target Dose, C",'Plot Data'!$B$13,"\\APPLEPI_AF\MWRD_Production\Hite Treatment Plant\07-Disinfection\Dis_PAA\North_PAA\North_PAA_Dose_Cntrl\CT Dosing Method","interpolated")</f>
+        <v>1.2999999523162842</v>
+      </c>
+      <c r="D13" s="44">
+        <f>AVERAGE(D14:D24)</f>
+        <v>54.113268071954899</v>
+      </c>
+      <c r="E13" s="44">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>1.2969*EXP(-0.16*E13)</f>
+        <v>1.2968999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="41">
+        <v>43600.387499999997</v>
+      </c>
+      <c r="C14" s="18">
+        <v>0.82</v>
+      </c>
+      <c r="D14" s="42">
+        <f t="array" ref="D14:D24">_xll.PITimeDat("N CMPLX OUTFALL WEIR (FI-F350)",'Plot Data'!$B$14:$B$24,"\\APPLEPI_AF\MWRD_Production\Hite Treatment Plant\07-Disinfection\Dis_Plant_Flows","interpolated")</f>
+        <v>60.482887268066406</v>
+      </c>
+      <c r="E14" s="44">
+        <v>2.9139740845546025</v>
+      </c>
+      <c r="G14">
+        <f>1.2969*EXP(-0.16*E14)</f>
+        <v>0.81362227836416889</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ref="H14:H24" si="2">0.8711*EXP(-0.029*E14)</f>
+        <v>0.80051200753881868</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="41">
+        <v>43600.385416666664</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.64</v>
+      </c>
+      <c r="D15" s="42">
+        <v>58.705768585205078</v>
+      </c>
+      <c r="E15">
+        <f>E14+(E17-E14)/2</f>
+        <v>7.8642753775994958</v>
+      </c>
+      <c r="G15">
+        <f>0.8499*EXP(-0.028*E15)</f>
+        <v>0.68192452525082492</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="2"/>
+        <v>0.69345946965983196</v>
+      </c>
+      <c r="J15" s="42">
+        <f>_xll.PITimeDat("AI_K826",'Plot Data'!$B$15,"\\applepi","interpolated")</f>
+        <v>0.48027771711349487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="41">
+        <v>43600.383333333331</v>
+      </c>
+      <c r="C16" s="18">
+        <v>0.63</v>
+      </c>
+      <c r="D16" s="42">
+        <v>56.880718231201172</v>
+      </c>
+      <c r="E16">
+        <f>E15+(E17-E15)/2</f>
+        <v>10.339426024121941</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ref="G16:G24" si="3">0.8499*EXP(-0.028*E16)</f>
+        <v>0.6362647605123346</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="2"/>
+        <v>0.64542784735666103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="41">
+        <v>43600.380555555559</v>
+      </c>
+      <c r="C17" s="18">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="D17" s="42">
+        <v>54.447315216064453</v>
+      </c>
+      <c r="E17">
+        <f>E14+(E20-E14)/2</f>
+        <v>12.814576670644389</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>0.59366224630344999</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="2"/>
+        <v>0.60072307664613778</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="41">
+        <v>43600.379166666666</v>
+      </c>
+      <c r="C18" s="18">
+        <v>0.53</v>
+      </c>
+      <c r="D18" s="42">
+        <v>53.888572692871094</v>
+      </c>
+      <c r="E18">
+        <f>E17+(E19-E17)/2</f>
+        <v>15.289727317166834</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>0.55391227765351914</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="2"/>
+        <v>0.55911472722029476</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="41">
+        <v>43600.377083333333</v>
+      </c>
+      <c r="C19" s="18">
+        <v>0.49</v>
+      </c>
+      <c r="D19" s="42">
+        <v>53.154514312744141</v>
+      </c>
+      <c r="E19">
+        <f>E17+(E20-E17)/2</f>
+        <v>17.76487796368928</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>0.51682385606592729</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="2"/>
+        <v>0.52038832924470857</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="41">
+        <v>43600.375694444447</v>
+      </c>
+      <c r="C20" s="18">
+        <v>0.45</v>
+      </c>
+      <c r="D20" s="42">
+        <v>52.665142059326172</v>
+      </c>
+      <c r="E20" s="44">
+        <v>22.715179256734174</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>0.44993074742759159</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="2"/>
+        <v>0.45079675434812544</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="41">
+        <v>43600.37222222222</v>
+      </c>
+      <c r="C21" s="18">
+        <v>0.44</v>
+      </c>
+      <c r="D21" s="42">
+        <v>51.746376037597656</v>
+      </c>
+      <c r="E21">
+        <f>E20+(E22-E20)/2</f>
+        <v>31.994488967988367</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>0.34698203435064895</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="2"/>
+        <v>0.34443886022416831</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="41">
+        <v>43600.370138888888</v>
+      </c>
+      <c r="C22" s="18">
+        <v>0.34</v>
+      </c>
+      <c r="D22" s="42">
+        <v>51.470790863037109</v>
+      </c>
+      <c r="E22" s="44">
+        <v>41.27379867924256</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="3"/>
+        <v>0.26758902975727533</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="2"/>
+        <v>0.26317431811167491</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" s="41">
+        <v>43600.367361111108</v>
+      </c>
+      <c r="C23" s="18">
+        <v>0.16</v>
+      </c>
+      <c r="D23" s="42">
+        <v>51.103347778320313</v>
+      </c>
+      <c r="E23">
+        <f>E22+(E24-E22)/2</f>
+        <v>50.553108390496746</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="3"/>
+        <v>0.20636194891312271</v>
+      </c>
+      <c r="H23">
+        <f>0.8711*EXP(-0.029*E23)</f>
+        <v>0.20108277465692662</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" s="41">
+        <v>43600.362500000003</v>
+      </c>
+      <c r="C24" s="18">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="D24" s="42">
+        <v>50.700515747070313</v>
+      </c>
+      <c r="E24" s="44">
+        <v>59.832418101750925</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>0.15914424443278</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="2"/>
+        <v>0.15364068406770043</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F25" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25">
+        <f>4.46353+20.731</f>
+        <v>25.19453</v>
+      </c>
+      <c r="H25">
+        <f>24.7657</f>
+        <v>24.765699999999999</v>
+      </c>
+      <c r="I25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F28" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="G28" s="44">
+        <f>RSQ(G2:G24,C2:C24)</f>
+        <v>0.98553546496573263</v>
+      </c>
+      <c r="H28" s="44">
+        <f>RSQ(H2:H24,C2:C24)</f>
+        <v>0.9383876849447953</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C16"/>
+      <selection activeCell="A5" sqref="A5:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,14 +4768,14 @@
       <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="47"/>
+      <c r="F3" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="34"/>
+      <c r="G3" s="49"/>
       <c r="H3" t="s">
         <v>32</v>
       </c>
@@ -2363,7 +4837,7 @@
         <f>2733.6*H5^(-0.956)</f>
         <v>46.585397160463273</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="36">
         <v>0</v>
       </c>
     </row>
@@ -2581,7 +5055,7 @@
       <c r="G12" s="3">
         <v>10</v>
       </c>
-      <c r="H12" s="39">
+      <c r="H12" s="35">
         <v>58.1</v>
       </c>
       <c r="I12">
@@ -2611,7 +5085,7 @@
       <c r="G13" s="3">
         <v>19</v>
       </c>
-      <c r="H13" s="39">
+      <c r="H13" s="35">
         <v>58.1</v>
       </c>
       <c r="I13">
@@ -2641,7 +5115,7 @@
       <c r="G14" s="3">
         <v>27</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="35">
         <v>58.1</v>
       </c>
       <c r="I14">
@@ -2671,7 +5145,7 @@
       <c r="G15" s="3">
         <v>780</v>
       </c>
-      <c r="H15" s="39">
+      <c r="H15" s="35">
         <v>58.27</v>
       </c>
       <c r="I15">
@@ -2701,7 +5175,7 @@
       <c r="G16" s="3">
         <v>17</v>
       </c>
-      <c r="H16" s="39">
+      <c r="H16" s="35">
         <v>58.6</v>
       </c>
       <c r="I16">
@@ -2763,50 +5237,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G34"/>
+  <dimension ref="A3:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H47" sqref="H47"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="42" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42" t="s">
+      <c r="C3" s="50"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="42"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="50"/>
+      <c r="G3" s="39"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="31"/>
+      <c r="E4" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="F4" s="31" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="31"/>
+      <c r="H4" s="40">
+        <v>43600</v>
+      </c>
+      <c r="I4" s="40">
+        <v>43598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -2816,42 +5300,56 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="37">
+        <f t="shared" ref="D5:D15" si="0">C5/$C$16</f>
         <v>0</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" s="17" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="37">
+        <f t="shared" ref="G5:G15" si="1">F5/$F$16</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="37">
         <v>0.11</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="37">
         <f>B6/70.8*24*60</f>
         <v>2.2372881355932206</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="37">
+        <f t="shared" si="0"/>
+        <v>4.8672566371681422E-2</v>
+      </c>
+      <c r="E6">
         <v>0.11</v>
       </c>
-      <c r="E6" s="41">
-        <f>D6/58.1*24*60</f>
+      <c r="F6" s="37">
+        <f>E6/58.1*24*60</f>
         <v>2.7263339070567989</v>
       </c>
-      <c r="F6" s="18">
+      <c r="G6" s="37">
+        <f t="shared" si="1"/>
+        <v>4.8888888888888891E-2</v>
+      </c>
+      <c r="H6" s="18">
         <v>0.82</v>
       </c>
-      <c r="G6" s="18">
+      <c r="I6" s="18">
         <v>0.95</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
         <v>14</v>
       </c>
@@ -2863,22 +5361,30 @@
         <f>C6+(C9-C6)/2</f>
         <v>6.0508474576271194</v>
       </c>
-      <c r="D7">
-        <f>D6+(D9-D6)/2</f>
-        <v>0.29499999999999998</v>
+      <c r="D7" s="37">
+        <f t="shared" si="0"/>
+        <v>0.13163716814159293</v>
       </c>
       <c r="E7">
         <f>E6+(E9-E6)/2</f>
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="F7">
+        <f>F6+(F9-F6)/2</f>
         <v>7.3115318416523243</v>
       </c>
-      <c r="F7" s="18">
+      <c r="G7" s="37">
+        <f t="shared" si="1"/>
+        <v>0.13111111111111112</v>
+      </c>
+      <c r="H7" s="18">
         <v>0.64</v>
       </c>
-      <c r="G7" s="18">
+      <c r="I7" s="18">
         <v>0.69</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>15</v>
       </c>
@@ -2890,22 +5396,30 @@
         <f>C7+(C9-C7)/2</f>
         <v>7.9576271186440684</v>
       </c>
-      <c r="D8">
-        <f>D7+(D9-D7)/2</f>
-        <v>0.38749999999999996</v>
+      <c r="D8" s="37">
+        <f t="shared" si="0"/>
+        <v>0.17311946902654868</v>
       </c>
       <c r="E8">
         <f>E7+(E9-E7)/2</f>
+        <v>0.38749999999999996</v>
+      </c>
+      <c r="F8">
+        <f>F7+(F9-F7)/2</f>
         <v>9.604130808950087</v>
       </c>
-      <c r="F8" s="18">
+      <c r="G8" s="37">
+        <f t="shared" si="1"/>
+        <v>0.17222222222222222</v>
+      </c>
+      <c r="H8" s="18">
         <v>0.63</v>
       </c>
-      <c r="G8" s="18">
+      <c r="I8" s="18">
         <v>0.69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
@@ -2917,22 +5431,30 @@
         <f>C6+(C12-C6)/2</f>
         <v>9.8644067796610173</v>
       </c>
-      <c r="D9">
-        <f>D6+(D12-D6)/2</f>
-        <v>0.48</v>
+      <c r="D9" s="37">
+        <f t="shared" si="0"/>
+        <v>0.21460176991150445</v>
       </c>
       <c r="E9">
         <f>E6+(E12-E6)/2</f>
+        <v>0.48</v>
+      </c>
+      <c r="F9">
+        <f>F6+(F12-F6)/2</f>
         <v>11.896729776247849</v>
       </c>
-      <c r="F9" s="18">
+      <c r="G9" s="37">
+        <f t="shared" si="1"/>
+        <v>0.21333333333333332</v>
+      </c>
+      <c r="H9" s="18">
         <v>0.56999999999999995</v>
       </c>
-      <c r="G9" s="18">
+      <c r="I9" s="18">
         <v>0.67</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
@@ -2944,22 +5466,30 @@
         <f>C9+(C11-C9)/2</f>
         <v>11.771186440677965</v>
       </c>
-      <c r="D10">
-        <f>D9+(D11-D9)/2</f>
-        <v>0.57250000000000001</v>
+      <c r="D10" s="37">
+        <f t="shared" si="0"/>
+        <v>0.25608407079646017</v>
       </c>
       <c r="E10">
         <f>E9+(E11-E9)/2</f>
+        <v>0.57250000000000001</v>
+      </c>
+      <c r="F10">
+        <f>F9+(F11-F9)/2</f>
         <v>14.189328743545611</v>
       </c>
-      <c r="F10" s="18">
+      <c r="G10" s="37">
+        <f t="shared" si="1"/>
+        <v>0.25444444444444442</v>
+      </c>
+      <c r="H10" s="18">
         <v>0.53</v>
       </c>
-      <c r="G10" s="18">
+      <c r="I10" s="18">
         <v>0.63</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
@@ -2971,47 +5501,63 @@
         <f>C9+(C12-C9)/2</f>
         <v>13.677966101694915</v>
       </c>
-      <c r="D11">
-        <f>D9+(D12-D9)/2</f>
-        <v>0.66500000000000004</v>
+      <c r="D11" s="37">
+        <f t="shared" si="0"/>
+        <v>0.29756637168141592</v>
       </c>
       <c r="E11">
         <f>E9+(E12-E9)/2</f>
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="F11">
+        <f>F9+(F12-F9)/2</f>
         <v>16.481927710843372</v>
       </c>
-      <c r="F11" s="18">
+      <c r="G11" s="37">
+        <f t="shared" si="1"/>
+        <v>0.29555555555555552</v>
+      </c>
+      <c r="H11" s="18">
         <v>0.49</v>
       </c>
-      <c r="G11" s="18">
+      <c r="I11" s="18">
         <v>0.62</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="41">
+      <c r="B12" s="37">
         <v>0.86</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C12" s="37">
         <f>B12/70.8*24*60</f>
         <v>17.491525423728813</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="37">
+        <f t="shared" si="0"/>
+        <v>0.38053097345132741</v>
+      </c>
+      <c r="E12">
         <v>0.85</v>
       </c>
-      <c r="E12" s="41">
-        <f>D12/58.1*24*60</f>
+      <c r="F12" s="37">
+        <f>E12/58.1*24*60</f>
         <v>21.0671256454389</v>
       </c>
-      <c r="F12" s="18">
+      <c r="G12" s="37">
+        <f t="shared" si="1"/>
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="H12" s="18">
         <v>0.45</v>
       </c>
-      <c r="G12" s="18">
+      <c r="I12" s="18">
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>22</v>
       </c>
@@ -3023,44 +5569,60 @@
         <f>C12+(C14-C12)/2</f>
         <v>24.610169491525426</v>
       </c>
-      <c r="D13">
-        <f>D12+(D14-D12)/2</f>
-        <v>1.2</v>
+      <c r="D13" s="37">
+        <f t="shared" si="0"/>
+        <v>0.53539823008849563</v>
       </c>
       <c r="E13">
         <f>E12+(E14-E12)/2</f>
+        <v>1.2</v>
+      </c>
+      <c r="F13">
+        <f>F12+(F14-F12)/2</f>
         <v>29.741824440619624</v>
       </c>
-      <c r="F13" s="18">
+      <c r="G13" s="37">
+        <f t="shared" si="1"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="H13" s="18">
         <v>0.44</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="41">
+      <c r="B14" s="37">
         <v>1.56</v>
       </c>
-      <c r="C14" s="41">
+      <c r="C14" s="37">
         <f>B14/70.8*24*60</f>
         <v>31.728813559322042</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="37">
+        <f t="shared" si="0"/>
+        <v>0.6902654867256639</v>
+      </c>
+      <c r="E14">
         <v>1.55</v>
       </c>
-      <c r="E14" s="41">
-        <f>D14/58.1*24*60</f>
+      <c r="F14" s="37">
+        <f>E14/58.1*24*60</f>
         <v>38.416523235800348</v>
       </c>
-      <c r="F14" s="18">
+      <c r="G14" s="37">
+        <f t="shared" si="1"/>
+        <v>0.68888888888888888</v>
+      </c>
+      <c r="H14" s="18">
         <v>0.34</v>
       </c>
-      <c r="G14" s="18">
+      <c r="I14" s="18">
         <v>0.47</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>23</v>
       </c>
@@ -3072,121 +5634,151 @@
         <f>C14+(C16-C14)/2</f>
         <v>38.847457627118644</v>
       </c>
-      <c r="D15">
-        <f>D14+(D16-D14)/2</f>
-        <v>1.9</v>
+      <c r="D15" s="37">
+        <f t="shared" si="0"/>
+        <v>0.84513274336283184</v>
       </c>
       <c r="E15">
         <f>E14+(E16-E14)/2</f>
+        <v>1.9</v>
+      </c>
+      <c r="F15">
+        <f>F14+(F16-F14)/2</f>
         <v>47.091222030981072</v>
       </c>
-      <c r="F15" s="18">
+      <c r="G15" s="37">
+        <f t="shared" si="1"/>
+        <v>0.84444444444444444</v>
+      </c>
+      <c r="H15" s="18">
         <v>0.16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="37">
         <v>2.2599999999999998</v>
       </c>
-      <c r="C16" s="41">
+      <c r="C16" s="37">
         <f>B16/70.8*24*60</f>
         <v>45.966101694915253</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="37">
+        <f>C16/$C$16</f>
+        <v>1</v>
+      </c>
+      <c r="E16">
         <v>2.25</v>
       </c>
-      <c r="E16" s="41">
-        <f>D16/58.1*24*60</f>
+      <c r="F16" s="37">
+        <f>E16/58.1*24*60</f>
         <v>55.765920826161796</v>
       </c>
-      <c r="F16" s="18">
+      <c r="G16" s="37">
+        <f>F16/$F$16</f>
+        <v>1</v>
+      </c>
+      <c r="H16" s="18">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G16" s="18">
+      <c r="I16" s="18">
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="14"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="13" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="36"/>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="37"/>
-      <c r="B29" s="38"/>
-      <c r="C29" s="38"/>
-      <c r="D29" s="38"/>
-      <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="37"/>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="37"/>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="37"/>
-      <c r="B32" s="38"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="38"/>
-      <c r="F32" s="38"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
-      <c r="B33" s="38"/>
-      <c r="C33" s="38"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="38"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="33"/>
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="33"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="33"/>
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="33"/>
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="33"/>
+      <c r="B33" s="34"/>
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="34"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="34"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="33"/>
+      <c r="B34" s="34"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="34"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>